<commit_message>
Added script to pull data from icici direct equity
</commit_message>
<xml_diff>
--- a/data/normalized/mdm.xlsx
+++ b/data/normalized/mdm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arun/repos/arunvambur/personal-analytics/data/normalized/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35DFFD6-7594-9548-B4E3-E401ED677E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E69880-7855-D748-9561-E5293D69516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17800" activeTab="6" xr2:uid="{0D9B0028-07D1-7947-A175-A21F9F058AC3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17800" activeTab="1" xr2:uid="{0D9B0028-07D1-7947-A175-A21F9F058AC3}"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6966" uniqueCount="669">
   <si>
     <t>Person</t>
   </si>
@@ -2005,6 +2005,81 @@
   </si>
   <si>
     <t>FT-FRSB INT DEC24 TBICI007109242</t>
+  </si>
+  <si>
+    <t>ICICI Breeze Code</t>
+  </si>
+  <si>
+    <t>AXIBAN</t>
+  </si>
+  <si>
+    <t>BANMAH</t>
+  </si>
+  <si>
+    <t>BOSLIM</t>
+  </si>
+  <si>
+    <t>CMSIN</t>
+  </si>
+  <si>
+    <t>COFDAY</t>
+  </si>
+  <si>
+    <t>DCXSYS</t>
+  </si>
+  <si>
+    <t>HDFBAN</t>
+  </si>
+  <si>
+    <t>ICIBAN</t>
+  </si>
+  <si>
+    <t>IDFBAN</t>
+  </si>
+  <si>
+    <t>INDIBA</t>
+  </si>
+  <si>
+    <t>INDHOT</t>
+  </si>
+  <si>
+    <t>INFTEC</t>
+  </si>
+  <si>
+    <t>INDRAI</t>
+  </si>
+  <si>
+    <t>ITCHOT</t>
+  </si>
+  <si>
+    <t>JAIPOW</t>
+  </si>
+  <si>
+    <t>LTFINA</t>
+  </si>
+  <si>
+    <t>LARTOU</t>
+  </si>
+  <si>
+    <t>OLAELE</t>
+  </si>
+  <si>
+    <t>SIEENE</t>
+  </si>
+  <si>
+    <t>SIEMEN</t>
+  </si>
+  <si>
+    <t>SUZENE</t>
+  </si>
+  <si>
+    <t>TATCOV</t>
+  </si>
+  <si>
+    <t>TATMOT</t>
+  </si>
+  <si>
+    <t>TATSTE</t>
   </si>
 </sst>
 </file>
@@ -2642,7 +2717,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -2699,6 +2774,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2745,7 +2822,35 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="&quot;₹&quot;#,##0.00"/>
     </dxf>
@@ -3077,7 +3182,7 @@
     <tableColumn id="1" xr3:uid="{10DE9821-BB62-9540-A58A-122CAD3F3AC3}" name="Id"/>
     <tableColumn id="2" xr3:uid="{D7E69AE7-23BC-174F-AB3D-BDF91431CD90}" name="Name"/>
     <tableColumn id="3" xr3:uid="{F229D4DB-0EDD-F64F-A22F-7E9FEF7A10BF}" name="DisplayName"/>
-    <tableColumn id="4" xr3:uid="{50FE2904-3015-5B45-9140-2F1B384AD178}" name="Dob" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{50FE2904-3015-5B45-9140-2F1B384AD178}" name="Dob" dataDxfId="40"/>
     <tableColumn id="5" xr3:uid="{FF9E5EB0-AFB8-A946-A83B-11BAFA15FE56}" name="GenderId"/>
     <tableColumn id="6" xr3:uid="{760A2E5F-6C0B-7E42-AA60-E6E3B078F34C}" name="IsFamilyHead"/>
     <tableColumn id="7" xr3:uid="{F955C30D-D2A1-F745-A684-FB311C4A3BC5}" name="FamilyHead"/>
@@ -3111,12 +3216,12 @@
     <tableColumn id="1" xr3:uid="{1019A78D-FD88-274C-ADF7-D0B577CAF779}" name="Person"/>
     <tableColumn id="2" xr3:uid="{0C2F4C8F-C5C1-BB47-A5C8-8CA089D9554B}" name="Account"/>
     <tableColumn id="3" xr3:uid="{032CAA0E-3C9A-C74A-BEE2-1991D924B223}" name="Pran"/>
-    <tableColumn id="4" xr3:uid="{66E6423A-FFFD-5E40-A617-D3D427E17E92}" name="Contribution Date" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{1682400D-E90F-6F47-9162-0DD08B859326}" name="Self Contribution" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{AED5945E-6CA4-2547-9F20-F440E51D273F}" name="Gross Contribution Amount" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{BB38DA8A-92AE-9747-AB7D-C7A9255159E3}" name="Service Charges" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{12F59806-4C0F-9F43-81F2-A0B24BAC055A}" name="GST" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{2CB0527E-E725-E446-88E4-053381A9500E}" name="Net Contribution Amount" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{66E6423A-FFFD-5E40-A617-D3D427E17E92}" name="Contribution Date" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{1682400D-E90F-6F47-9162-0DD08B859326}" name="Self Contribution" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{AED5945E-6CA4-2547-9F20-F440E51D273F}" name="Gross Contribution Amount" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{BB38DA8A-92AE-9747-AB7D-C7A9255159E3}" name="Service Charges" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{12F59806-4C0F-9F43-81F2-A0B24BAC055A}" name="GST" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{2CB0527E-E725-E446-88E4-053381A9500E}" name="Net Contribution Amount" dataDxfId="5"/>
     <tableColumn id="12" xr3:uid="{DE3D2D83-5648-0B43-8EA8-6243CE3B3EB0}" name="Account Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3129,12 +3234,12 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{AA226644-822D-0144-80ED-9B295E5C69CC}" name="Person"/>
     <tableColumn id="2" xr3:uid="{85819774-7B4A-8A48-8235-C5A97D157FE1}" name="Account"/>
-    <tableColumn id="3" xr3:uid="{1FAD624B-EFC7-8B44-A1A2-B2B431400749}" name="Date" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{2DAFC7E5-D2A1-C84D-91CA-590F1D2D8AE8}" name="Type" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1FAD624B-EFC7-8B44-A1A2-B2B431400749}" name="Date" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{2DAFC7E5-D2A1-C84D-91CA-590F1D2D8AE8}" name="Type" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{E21CFFCC-B366-AF4C-9429-07B760EB6AD7}" name="Scheme"/>
     <tableColumn id="9" xr3:uid="{9D4E1016-5E5A-7B41-AE4B-DFCD445AD6D4}" name="Particulars"/>
     <tableColumn id="6" xr3:uid="{CE9A0357-2B9E-C04C-9B44-E2D25E7F28F5}" name="Rate of Interest"/>
-    <tableColumn id="7" xr3:uid="{2DA438FA-E99D-0746-801C-DFB9D8F8A6B7}" name="Amount" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{2DA438FA-E99D-0746-801C-DFB9D8F8A6B7}" name="Amount" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{E529750B-EC3E-CD41-B54B-F2F30B0D043D}" name="Marutiry Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3142,18 +3247,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{3478D0AF-1514-EB4A-8A5D-C5ECD02546DB}" name="ISINTable" displayName="ISINTable" ref="A1:F31" headerRowDxfId="37" dataDxfId="36" totalsRowDxfId="35">
-  <autoFilter ref="A1:F31" xr:uid="{3478D0AF-1514-EB4A-8A5D-C5ECD02546DB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{3478D0AF-1514-EB4A-8A5D-C5ECD02546DB}" name="ISINTable" displayName="ISINTable" ref="A1:G31" headerRowDxfId="39" dataDxfId="38" totalsRowDxfId="37">
+  <autoFilter ref="A1:G31" xr:uid="{3478D0AF-1514-EB4A-8A5D-C5ECD02546DB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D31">
     <sortCondition ref="B2:B31"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C91CFA9A-AB89-9341-9F89-D481613B35F0}" name="ISIN" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{94B85035-7256-DF49-A14F-D99830860AAE}" name="Company" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{1FAF0D6D-A333-C14D-8320-F5B0EEC2AFF8}" name="NSE Symbol" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{0969A61B-61F8-2A43-9C8D-745D74851EA3}" name="BSE Code" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{F59184CE-A708-4B46-AAA4-9119706B3E96}" name="Incorporation Date" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{3F95A63A-F7FB-0F44-A472-49446749F45E}" name="ISIN Creation Date" dataDxfId="28" totalsRowDxfId="27"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{C91CFA9A-AB89-9341-9F89-D481613B35F0}" name="ISIN" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{94B85035-7256-DF49-A14F-D99830860AAE}" name="Company" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{1FAF0D6D-A333-C14D-8320-F5B0EEC2AFF8}" name="NSE Symbol" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{0969A61B-61F8-2A43-9C8D-745D74851EA3}" name="BSE Code" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{F59184CE-A708-4B46-AAA4-9119706B3E96}" name="Incorporation Date" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{3F95A63A-F7FB-0F44-A472-49446749F45E}" name="ISIN Creation Date" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{E11E9DC1-916F-114C-991E-73874650D707}" name="ICICI Breeze Code" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3165,7 +3271,7 @@
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{402B9537-46B3-D440-B7E5-FB14BE83DAEC}" name="Person"/>
     <tableColumn id="2" xr3:uid="{27B331BE-0616-4343-992A-640D2131D6EE}" name="Account"/>
-    <tableColumn id="3" xr3:uid="{F8C0F30E-0A07-454A-98E4-2A39D664C705}" name="Trade Date" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{F8C0F30E-0A07-454A-98E4-2A39D664C705}" name="Trade Date" dataDxfId="28"/>
     <tableColumn id="4" xr3:uid="{F66FD8B2-E1FB-9747-8FAC-221378536716}" name="ISIN"/>
     <tableColumn id="5" xr3:uid="{AB3B46B3-3390-A24B-88BF-711CB56D2780}" name="Security"/>
     <tableColumn id="6" xr3:uid="{5412213A-12EC-8941-A589-C643C34E10EB}" name="Segment"/>
@@ -3191,7 +3297,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{92851E3D-CC2E-2646-9CDE-D7F28D8FA284}" name="Table15" displayName="Table15" ref="A1:N151" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{92851E3D-CC2E-2646-9CDE-D7F28D8FA284}" name="Table15" displayName="Table15" ref="A1:N151" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="A1:N151" xr:uid="{92851E3D-CC2E-2646-9CDE-D7F28D8FA284}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N151">
     <sortCondition ref="C2:C151"/>
@@ -3199,16 +3305,16 @@
   <tableColumns count="14">
     <tableColumn id="12" xr3:uid="{3840908B-FF83-CB41-AAE2-5035AE6E16C0}" name="People"/>
     <tableColumn id="1" xr3:uid="{6FD593F6-C345-974D-933D-FC749EDBB157}" name="Record Date"/>
-    <tableColumn id="2" xr3:uid="{15AD3D5E-EF83-6546-A4FE-0B86CA16CA88}" name="Date" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{15AD3D5E-EF83-6546-A4FE-0B86CA16CA88}" name="Date" dataDxfId="26"/>
     <tableColumn id="3" xr3:uid="{1ED970B8-C337-5D4F-B5A8-7AB2530E2359}" name="Account"/>
     <tableColumn id="4" xr3:uid="{EEAA2927-43F1-B744-8527-40D0D0E9936D}" name="ISIN"/>
     <tableColumn id="5" xr3:uid="{0EA1DB11-9FE8-934D-B07C-6945A710E2FD}" name="Stock"/>
     <tableColumn id="6" xr3:uid="{272913E2-1E54-2C45-80CD-6843C57552CE}" name="Nature"/>
     <tableColumn id="7" xr3:uid="{79D5F1AE-2819-AE4A-8B96-282AE4111C82}" name="Quantity"/>
-    <tableColumn id="8" xr3:uid="{DADE57C5-0E46-6746-A0AB-0C9AAB41E9E2}" name="Per Share" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{B575C695-6DE9-B146-9ED9-368D32B0C729}" name="Ratio" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{403EF57C-A4F3-7C4E-A4C6-5D54E2D0E2A8}" name="Dividend Amount" dataDxfId="21"/>
-    <tableColumn id="14" xr3:uid="{D5C383E4-A206-2D40-974E-4A42225ED82E}" name="Total Units" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{DADE57C5-0E46-6746-A0AB-0C9AAB41E9E2}" name="Per Share" dataDxfId="25"/>
+    <tableColumn id="13" xr3:uid="{B575C695-6DE9-B146-9ED9-368D32B0C729}" name="Ratio" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{403EF57C-A4F3-7C4E-A4C6-5D54E2D0E2A8}" name="Dividend Amount" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{D5C383E4-A206-2D40-974E-4A42225ED82E}" name="Total Units" dataDxfId="22"/>
     <tableColumn id="10" xr3:uid="{71D272A4-B312-8C4C-B946-831230DC7CB7}" name="TaxOnDividend"/>
     <tableColumn id="11" xr3:uid="{48F92846-C887-5340-9893-9723B5AB06B5}" name="FinalAmount"/>
   </tableColumns>
@@ -3218,24 +3324,18 @@
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{413EE8ED-1C2E-6844-82BF-A265CD4C35A6}" name="Table3" displayName="Table3" ref="A1:Q273" totalsRowShown="0">
-  <autoFilter ref="A1:Q273" xr:uid="{413EE8ED-1C2E-6844-82BF-A265CD4C35A6}">
-    <filterColumn colId="14">
-      <filters>
-        <filter val="Executed"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q273" xr:uid="{413EE8ED-1C2E-6844-82BF-A265CD4C35A6}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{749626B5-F3F2-3945-B121-B98CB0A96B1E}" name="Person"/>
     <tableColumn id="2" xr3:uid="{706C6171-6C85-4944-AE29-D3C3F3583B72}" name="Account"/>
-    <tableColumn id="3" xr3:uid="{A2D40B47-4967-C64A-9182-091485684E6A}" name="Date" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{A2D40B47-4967-C64A-9182-091485684E6A}" name="Date" dataDxfId="21"/>
     <tableColumn id="4" xr3:uid="{5BCFE48E-58D1-A94C-B817-263D47389785}" name="Transaction ID"/>
     <tableColumn id="5" xr3:uid="{FD7B050B-A92C-044A-945B-4C77F389712E}" name="Transaction Type"/>
     <tableColumn id="6" xr3:uid="{4D6D2013-C60A-0E4F-B241-2AE9EE90CBB1}" name="Fund Name"/>
     <tableColumn id="7" xr3:uid="{0A1516F9-7859-C14A-816A-5BB2BD9EADEA}" name="Scheme Name"/>
     <tableColumn id="8" xr3:uid="{1D393BA1-453A-DF4C-8D45-89BA94B67277}" name="Folio No"/>
     <tableColumn id="9" xr3:uid="{56F26D36-AE6D-AD46-89E4-A7852A8C0009}" name="Last recorded NAV"/>
-    <tableColumn id="10" xr3:uid="{D6D71F70-1357-D946-B9F9-7BBF85DEB1E9}" name="Last recorded NAV On" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{D6D71F70-1357-D946-B9F9-7BBF85DEB1E9}" name="Last recorded NAV On" dataDxfId="20"/>
     <tableColumn id="11" xr3:uid="{6EF90D28-A94E-E746-9638-3F9E3EA4EE99}" name="Div-Reinvestment"/>
     <tableColumn id="12" xr3:uid="{897CE7E2-4A44-594A-A5FF-D9179111CFE9}" name="Amount"/>
     <tableColumn id="13" xr3:uid="{4C2F8C3E-95CF-1E4A-AD08-106718EDA162}" name="Secure Mind Premium Amount"/>
@@ -3255,8 +3355,8 @@
     <sortCondition ref="E2:E144"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{D24591B3-E216-8D40-A95C-7791798C856E}" name="Person " dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{226C7B2A-0A5E-4343-A7C2-ACEF96718284}" name="Account" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{D24591B3-E216-8D40-A95C-7791798C856E}" name="Person " dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{226C7B2A-0A5E-4343-A7C2-ACEF96718284}" name="Account" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{9BE64CD6-5BC7-C54A-8A02-A5602AE728A2}" name="AMC Name"/>
     <tableColumn id="4" xr3:uid="{3F1FB83B-D23F-3244-A7AB-6265DD4F5BF2}" name="Scheme Name"/>
     <tableColumn id="5" xr3:uid="{2B304844-D1AD-0F4C-9F20-58C883CB558E}" name="Record Date"/>
@@ -3265,7 +3365,7 @@
     <tableColumn id="8" xr3:uid="{DE9A2840-5F21-F74A-921B-D177FE4100BB}" name="Gross Amount(rs.)"/>
     <tableColumn id="9" xr3:uid="{A054CBE3-A57C-B341-9F81-737DE8A75663}" name="Units"/>
     <tableColumn id="10" xr3:uid="{4135883F-DFC4-0148-B9A4-0D963DBF04A8}" name="Dividend Type"/>
-    <tableColumn id="11" xr3:uid="{0848FCA6-35D7-094C-AF33-22A1FFBA89F4}" name=" Missing Date" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{0848FCA6-35D7-094C-AF33-22A1FFBA89F4}" name=" Missing Date" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3278,8 +3378,8 @@
     <tableColumn id="1" xr3:uid="{23163881-7E31-7B46-A375-9FB555FE9CD7}" name="Person"/>
     <tableColumn id="2" xr3:uid="{AAD497D8-F3B6-D04C-A94C-DDA752626E57}" name="Policy No"/>
     <tableColumn id="3" xr3:uid="{6C32D55C-8827-A842-ADDB-A6CB32AA543A}" name="Agency Code"/>
-    <tableColumn id="4" xr3:uid="{EC651C3D-5628-894C-919A-2B9418E32725}" name="Premium Due Date" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{CF3189AE-A91A-CB44-978F-0F17593743CF}" name="Paid on" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{EC651C3D-5628-894C-919A-2B9418E32725}" name="Premium Due Date" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{CF3189AE-A91A-CB44-978F-0F17593743CF}" name="Paid on" dataDxfId="15"/>
     <tableColumn id="6" xr3:uid="{A0C51315-5F64-6043-AF0C-64D2AEB2BA7E}" name="Transaction No"/>
     <tableColumn id="7" xr3:uid="{8C082829-0673-3C49-9ED9-16A2400DF679}" name="Transaction Type"/>
     <tableColumn id="8" xr3:uid="{90542E0C-78F8-3C44-AB2D-BC24A080C513}" name="Premium Amount"/>
@@ -3310,7 +3410,7 @@
     <tableColumn id="4" xr3:uid="{8E2B2B65-A750-534D-A85F-9A9001313E51}" name="Member ID"/>
     <tableColumn id="5" xr3:uid="{84942EA2-D70B-9548-8B23-2350F3695C55}" name="Year"/>
     <tableColumn id="6" xr3:uid="{0F8059C3-D672-E24A-8C98-AEF8CDBD3FFE}" name="Transaction Type"/>
-    <tableColumn id="7" xr3:uid="{F041853A-9AB0-3346-AFEE-B4E9866D8A53}" name="Date" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{F041853A-9AB0-3346-AFEE-B4E9866D8A53}" name="Date" dataDxfId="14"/>
     <tableColumn id="8" xr3:uid="{70F0825D-EA40-AD49-BD29-98BEEB0A1A0D}" name="Particulars"/>
     <tableColumn id="9" xr3:uid="{658A6304-2B1B-5348-8085-A978F2B8EB96}" name="Wages"/>
     <tableColumn id="10" xr3:uid="{3B30A7FA-DB79-AE4F-98BE-03A63154072C}" name="Contribution"/>
@@ -3328,9 +3428,9 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7711BE01-18A6-8C47-B9F5-454678DCF505}" name="Person"/>
     <tableColumn id="2" xr3:uid="{6E8EF78F-DE19-944F-9D42-EF9C41943A33}" name="Financial Year"/>
-    <tableColumn id="3" xr3:uid="{38672957-E911-6649-ADA3-70D4C9727659}" name="Date" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{65B8E558-D743-9D4C-803B-DC44ACF8623B}" name="Particulars" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{C51610E1-510B-054C-9702-39FC1135D5D2}" name="Amount" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{38672957-E911-6649-ADA3-70D4C9727659}" name="Date" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{65B8E558-D743-9D4C-803B-DC44ACF8623B}" name="Particulars" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{C51610E1-510B-054C-9702-39FC1135D5D2}" name="Amount" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{4A162B93-7283-354A-B65F-A8A767DCF522}" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6699,10 +6799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB37A14D-5252-7042-8972-F4D6E9228613}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6713,9 +6813,10 @@
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -6734,8 +6835,11 @@
       <c r="F1" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="38" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -6751,8 +6855,11 @@
       <c r="E2" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="38" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -6768,8 +6875,11 @@
       <c r="E3" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="38" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>157</v>
       </c>
@@ -6785,8 +6895,11 @@
       <c r="E4" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="38" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -6802,8 +6915,11 @@
       <c r="E5" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="38" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -6819,8 +6935,11 @@
       <c r="E6" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="38" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -6839,8 +6958,11 @@
       <c r="F7" s="1">
         <v>44876</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="38" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -6856,8 +6978,11 @@
       <c r="E8" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="38" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -6876,8 +7001,11 @@
       <c r="F9" s="1">
         <v>34845</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="38" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -6893,8 +7021,11 @@
       <c r="E10" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="38" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -6910,8 +7041,11 @@
       <c r="E11" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="38" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -6930,8 +7064,11 @@
       <c r="F12" s="1">
         <v>43752</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="38" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -6950,8 +7087,11 @@
       <c r="F13" s="1">
         <v>44497</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="38" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -6970,8 +7110,11 @@
       <c r="F14" s="1">
         <v>45686</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="38" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>478</v>
       </c>
@@ -6987,8 +7130,11 @@
       <c r="E15" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="38" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -7004,8 +7150,11 @@
       <c r="E16" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="38" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>159</v>
       </c>
@@ -7021,8 +7170,11 @@
       <c r="E17" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="38" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>156</v>
       </c>
@@ -7038,8 +7190,11 @@
       <c r="E18" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>150</v>
       </c>
@@ -7055,8 +7210,11 @@
       <c r="E19" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="38" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -7072,8 +7230,11 @@
       <c r="E20" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="38" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -7089,8 +7250,11 @@
       <c r="E21" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" s="38" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -7106,8 +7270,11 @@
       <c r="E22" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" s="38" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>148</v>
       </c>
@@ -7126,8 +7293,11 @@
       <c r="F23" s="1">
         <v>45513</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="38" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -7146,8 +7316,11 @@
       <c r="F24" s="1">
         <v>45827</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="38" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>446</v>
       </c>
@@ -7163,8 +7336,11 @@
       <c r="E25" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" s="38" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -7180,8 +7356,11 @@
       <c r="E26" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -7200,13 +7379,16 @@
       <c r="F27" s="1">
         <v>45303</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" s="38" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>506</v>
+        <v>546</v>
       </c>
       <c r="C28" t="s">
         <v>41</v>
@@ -7218,13 +7400,16 @@
         <v>545</v>
       </c>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" s="38" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>67</v>
       </c>
-      <c r="B29" t="s">
-        <v>546</v>
+      <c r="B29" s="39" t="s">
+        <v>506</v>
       </c>
       <c r="C29" t="s">
         <v>473</v>
@@ -7238,8 +7423,11 @@
       <c r="F29" s="1">
         <v>45839</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" s="38" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -7256,8 +7444,11 @@
         <v>548</v>
       </c>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="38" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -7276,9 +7467,13 @@
       <c r="F31" s="1">
         <v>44770</v>
       </c>
+      <c r="G31" s="38" t="s">
+        <v>668</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -7289,7 +7484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913D0F15-B5AF-2B43-8EE8-D5A767C72F77}">
   <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
@@ -16715,7 +16910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E490D1BC-2804-2F4B-A84D-0FDC669319C7}">
   <dimension ref="A1:S273"/>
   <sheetViews>
-    <sheetView topLeftCell="A251" workbookViewId="0">
+    <sheetView topLeftCell="A250" workbookViewId="0">
       <selection activeCell="F274" sqref="F274"/>
     </sheetView>
   </sheetViews>
@@ -18154,7 +18349,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:17" hidden="1">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -18404,7 +18599,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:17" hidden="1">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -29904,7 +30099,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="264" spans="1:17" hidden="1">
+    <row r="264" spans="1:17">
       <c r="A264" t="s">
         <v>82</v>
       </c>
@@ -30416,7 +30611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82AF4798-4406-9B45-98C1-81D349601EE7}">
   <dimension ref="A1:K196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+    <sheetView topLeftCell="A171" workbookViewId="0">
       <selection activeCell="D197" sqref="D197"/>
     </sheetView>
   </sheetViews>

</xml_diff>